<commit_message>
Extra sheet on Excel brief
</commit_message>
<xml_diff>
--- a/Brief/Brief.xlsx
+++ b/Brief/Brief.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A54C2D05-6A5B-4667-AEFA-1BE8865C5BC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B28D2099-9C61-49A6-9DDE-6822BDFECC7F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stracture" sheetId="1" r:id="rId1"/>
     <sheet name="Info" sheetId="2" r:id="rId2"/>
+    <sheet name="Extra" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_1hljhzhi7rkj" localSheetId="0">Stracture!$B$16</definedName>
@@ -985,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1435,4 +1436,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CE9ABC-C43C-4B06-B7AF-247A530B21C3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>